<commit_message>
update dataset, analysis, plot, and add requirements
</commit_message>
<xml_diff>
--- a/DATASET.xlsx
+++ b/DATASET.xlsx
@@ -5,16 +5,17 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jessica\VsCode\Skripsi\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jessica\VsCode\clustering-tpt-tpak\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B517630F-8A48-4C98-937F-6A0C2627DFEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E6D1523-7DE0-44D4-AC96-38B097317C91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Populasi" sheetId="1" r:id="rId1"/>
-    <sheet name="Sampel" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId2"/>
+    <sheet name="Sampel" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="94">
   <si>
     <t>No</t>
   </si>
@@ -126,9 +127,6 @@
     <t>Kota Gunungsitoli</t>
   </si>
   <si>
-    <t>Kota Padangsidimpuan</t>
-  </si>
-  <si>
     <t>Pasangkayu</t>
   </si>
   <si>
@@ -145,9 +143,6 @@
   </si>
   <si>
     <t>Majene</t>
-  </si>
-  <si>
-    <t>Gorontalo</t>
   </si>
   <si>
     <t>Tojo Una Una</t>
@@ -279,9 +274,6 @@
     <t>Kota Parepare</t>
   </si>
   <si>
-    <t>Pangkajene Dan Kepulauan</t>
-  </si>
-  <si>
     <t>Sidenreng Rappang</t>
   </si>
   <si>
@@ -293,12 +285,48 @@
   <si>
     <t>Bangli</t>
   </si>
+  <si>
+    <t>Kota Metro</t>
+  </si>
+  <si>
+    <t>Kota Bandar Lampung</t>
+  </si>
+  <si>
+    <t>Kota Pangkal Pinang</t>
+  </si>
+  <si>
+    <t>Kota Gorontalo</t>
+  </si>
+  <si>
+    <t>Kota Ambon</t>
+  </si>
+  <si>
+    <t>Kota Ternate</t>
+  </si>
+  <si>
+    <t>Kota Padang Sidempuan</t>
+  </si>
+  <si>
+    <t>Kota Tanjung Balai</t>
+  </si>
+  <si>
+    <t>Kota Bontang</t>
+  </si>
+  <si>
+    <t>Kota Tual</t>
+  </si>
+  <si>
+    <t>Pangkajene Kepulauan</t>
+  </si>
+  <si>
+    <t>Kepulauan Siau Tagulandang Biaro</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -331,6 +359,12 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -369,7 +403,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -395,6 +429,9 @@
     <xf numFmtId="2" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -616,8 +653,8 @@
   </sheetPr>
   <dimension ref="A1:Q1000"/>
   <sheetViews>
-    <sheetView topLeftCell="A270" zoomScale="151" workbookViewId="0">
-      <selection activeCell="C277" sqref="C277"/>
+    <sheetView tabSelected="1" topLeftCell="B133" zoomScale="151" workbookViewId="0">
+      <selection activeCell="C141" sqref="C141"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -630,7 +667,7 @@
   <sheetData>
     <row r="1" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B1" s="1" t="str">
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"prov")</f>
@@ -2707,7 +2744,7 @@
         <v>SUMATERA UTARA</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D31" s="2">
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),6.98)</f>
@@ -3810,7 +3847,7 @@
         <v>SUMATERA UTARA</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D47" s="2">
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),5.67)</f>
@@ -4084,9 +4121,8 @@
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"SUMATERA UTARA")</f>
         <v>SUMATERA UTARA</v>
       </c>
-      <c r="C51" s="2" t="str">
-        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Tanjungbalai")</f>
-        <v>Tanjungbalai</v>
+      <c r="C51" s="10" t="s">
+        <v>89</v>
       </c>
       <c r="D51" s="2">
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),5.58)</f>
@@ -4425,8 +4461,8 @@
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"SUMATERA UTARA")</f>
         <v>SUMATERA UTARA</v>
       </c>
-      <c r="C56" s="2" t="s">
-        <v>29</v>
+      <c r="C56" s="10" t="s">
+        <v>88</v>
       </c>
       <c r="D56" s="2">
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),5.18)</f>
@@ -4561,8 +4597,8 @@
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"SUMATERA BARAT")</f>
         <v>SUMATERA BARAT</v>
       </c>
-      <c r="C58" s="2" t="s">
-        <v>67</v>
+      <c r="C58" s="10" t="s">
+        <v>65</v>
       </c>
       <c r="D58" s="2">
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),2.31)</f>
@@ -4630,7 +4666,7 @@
         <v>SUMATERA BARAT</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D59" s="2">
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),6.03)</f>
@@ -4698,7 +4734,7 @@
         <v>SUMATERA BARAT</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D60" s="2">
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),6.12)</f>
@@ -4766,7 +4802,7 @@
         <v>SUMATERA BARAT</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D61" s="2">
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),3.22)</f>
@@ -4834,7 +4870,7 @@
         <v>SUMATERA BARAT</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D62" s="2">
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),4.01)</f>
@@ -4902,7 +4938,7 @@
         <v>SUMATERA BARAT</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D63" s="2">
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),7.03)</f>
@@ -4970,7 +5006,7 @@
         <v>SUMATERA BARAT</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D64" s="2">
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),4.93)</f>
@@ -5038,7 +5074,7 @@
         <v>SUMATERA BARAT</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D65" s="2">
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),2.73)</f>
@@ -5106,7 +5142,7 @@
         <v>SUMATERA BARAT</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D66" s="2">
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),6.04)</f>
@@ -5174,7 +5210,7 @@
         <v>SUMATERA BARAT</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D67" s="2">
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),5.84)</f>
@@ -5242,7 +5278,7 @@
         <v>SUMATERA BARAT</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D68" s="2">
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),4.02)</f>
@@ -5310,7 +5346,7 @@
         <v>SUMATERA BARAT</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D69" s="2">
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),3.36)</f>
@@ -6551,7 +6587,7 @@
         <v>RIAU</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D87" s="2">
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),8.42)</f>
@@ -6876,7 +6912,7 @@
         <v>JAMBI</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D92" s="2">
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),3.87)</f>
@@ -7757,7 +7793,7 @@
         <v>SUMATERA SELATAN</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D106" s="2">
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),3.86)</f>
@@ -8386,7 +8422,7 @@
         <v>SUMATERA SELATAN</v>
       </c>
       <c r="C116" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D116" s="2">
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),4.59)</f>
@@ -8763,7 +8799,7 @@
         <v>BENGKULU</v>
       </c>
       <c r="C122" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D122" s="2">
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),4.73)</f>
@@ -9973,9 +10009,8 @@
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"LAMPUNG")</f>
         <v>LAMPUNG</v>
       </c>
-      <c r="C140" s="2" t="str">
-        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Bandar Lampung")</f>
-        <v>Bandar Lampung</v>
+      <c r="C140" s="10" t="s">
+        <v>83</v>
       </c>
       <c r="D140" s="2">
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),7.27)</f>
@@ -10042,9 +10077,8 @@
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"LAMPUNG")</f>
         <v>LAMPUNG</v>
       </c>
-      <c r="C141" s="2" t="str">
-        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Metro")</f>
-        <v>Metro</v>
+      <c r="C141" s="10" t="s">
+        <v>82</v>
       </c>
       <c r="D141" s="2">
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),5.79)</f>
@@ -10525,9 +10559,8 @@
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"BANGKA BELITUNG")</f>
         <v>BANGKA BELITUNG</v>
       </c>
-      <c r="C148" s="2" t="str">
-        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Pangkal Pinang")</f>
-        <v>Pangkal Pinang</v>
+      <c r="C148" s="10" t="s">
+        <v>84</v>
       </c>
       <c r="D148" s="2">
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),4.7)</f>
@@ -10910,7 +10943,7 @@
         <v>KEPULAUAN RIAU</v>
       </c>
       <c r="C154" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D154" s="2">
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),10.07)</f>
@@ -10972,7 +11005,7 @@
         <v>KEPULAUAN RIAU</v>
       </c>
       <c r="C155" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D155" s="2">
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),6)</f>
@@ -11034,7 +11067,7 @@
         <v>DKI JAKARTA</v>
       </c>
       <c r="C156" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D156" s="2">
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),6.06)</f>
@@ -11102,7 +11135,7 @@
         <v>DKI JAKARTA</v>
       </c>
       <c r="C157" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D157" s="2">
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),6.59)</f>
@@ -11170,7 +11203,7 @@
         <v>DKI JAKARTA</v>
       </c>
       <c r="C158" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D158" s="2">
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),7.13)</f>
@@ -11238,7 +11271,7 @@
         <v>DKI JAKARTA</v>
       </c>
       <c r="C159" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D159" s="2">
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),7.06)</f>
@@ -11306,7 +11339,7 @@
         <v>DKI JAKARTA</v>
       </c>
       <c r="C160" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D160" s="2">
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),5.42)</f>
@@ -11374,7 +11407,7 @@
         <v>DKI JAKARTA</v>
       </c>
       <c r="C161" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D161" s="2">
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),7.43)</f>
@@ -18687,7 +18720,7 @@
         <v>BANTEN</v>
       </c>
       <c r="C267" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D267" s="2">
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),8.19)</f>
@@ -18755,7 +18788,7 @@
         <v>BANTEN</v>
       </c>
       <c r="C268" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D268" s="2">
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),7.57)</f>
@@ -18823,7 +18856,7 @@
         <v>BANTEN</v>
       </c>
       <c r="C269" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D269" s="2">
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),9.63)</f>
@@ -18891,7 +18924,7 @@
         <v>BANTEN</v>
       </c>
       <c r="C270" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D270" s="2">
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),12.63)</f>
@@ -23927,7 +23960,7 @@
         <v>KALIMANTAN TENGAH</v>
       </c>
       <c r="C343" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D343" s="2">
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),5.77)</f>
@@ -24823,7 +24856,7 @@
         <v>KALIMANTAN SELATAN</v>
       </c>
       <c r="C356" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D356" s="2">
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),5.11)</f>
@@ -25332,7 +25365,7 @@
         <v>KALIMANTAN TIMUR</v>
       </c>
       <c r="C364" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D364" s="2">
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),9.27)</f>
@@ -25394,7 +25427,7 @@
         <v>KALIMANTAN TIMUR</v>
       </c>
       <c r="C365" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D365" s="2">
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),5.99)</f>
@@ -25455,9 +25488,8 @@
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"KALIMANTAN TIMUR")</f>
         <v>KALIMANTAN TIMUR</v>
       </c>
-      <c r="C366" s="2" t="str">
-        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Bontang")</f>
-        <v>Bontang</v>
+      <c r="C366" s="10" t="s">
+        <v>90</v>
       </c>
       <c r="D366" s="2">
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),9.41)</f>
@@ -25795,7 +25827,7 @@
         <v>KALIMANTAN UTARA</v>
       </c>
       <c r="C371" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D371" s="2">
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),5.89)</f>
@@ -26324,9 +26356,8 @@
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"SULAWESI UTARA")</f>
         <v>SULAWESI UTARA</v>
       </c>
-      <c r="C379" s="2" t="str">
-        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Kepulauan Sitaro")</f>
-        <v>Kepulauan Sitaro</v>
+      <c r="C379" s="2" t="s">
+        <v>93</v>
       </c>
       <c r="D379" s="2">
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),2.7)</f>
@@ -27198,7 +27229,7 @@
         <v>SULAWESI TENGAH</v>
       </c>
       <c r="C392" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D392" s="2">
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),3.18)</f>
@@ -27404,7 +27435,7 @@
         <v>SULAWESI TENGAH</v>
       </c>
       <c r="C395" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D395" s="2">
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),3.74)</f>
@@ -28299,8 +28330,8 @@
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"SULAWESI SELATAN")</f>
         <v>SULAWESI SELATAN</v>
       </c>
-      <c r="C408" s="2" t="s">
-        <v>80</v>
+      <c r="C408" s="10" t="s">
+        <v>92</v>
       </c>
       <c r="D408" s="2">
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),6.91)</f>
@@ -28644,7 +28675,7 @@
         <v>SULAWESI SELATAN</v>
       </c>
       <c r="C413" s="2" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D413" s="2">
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),4.7)</f>
@@ -29195,7 +29226,7 @@
         <v>SULAWESI SELATAN</v>
       </c>
       <c r="C421" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D421" s="2">
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),12.19)</f>
@@ -29263,7 +29294,7 @@
         <v>SULAWESI SELATAN</v>
       </c>
       <c r="C422" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D422" s="2">
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),6.81)</f>
@@ -29331,7 +29362,7 @@
         <v>SULAWESI SELATAN</v>
       </c>
       <c r="C423" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D423" s="2">
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),11.6)</f>
@@ -30886,8 +30917,8 @@
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"GORONTALO")</f>
         <v>GORONTALO</v>
       </c>
-      <c r="C446" s="2" t="s">
-        <v>36</v>
+      <c r="C446" s="10" t="s">
+        <v>85</v>
       </c>
       <c r="D446" s="2">
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),5.36)</f>
@@ -30949,7 +30980,7 @@
         <v>SULAWESI BARAT</v>
       </c>
       <c r="C447" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D447" s="2">
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),3.53)</f>
@@ -31017,7 +31048,7 @@
         <v>SULAWESI BARAT</v>
       </c>
       <c r="C448" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D448" s="2">
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),2.97)</f>
@@ -31085,7 +31116,7 @@
         <v>SULAWESI BARAT</v>
       </c>
       <c r="C449" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D449" s="2">
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),2.95)</f>
@@ -31153,7 +31184,7 @@
         <v>SULAWESI BARAT</v>
       </c>
       <c r="C450" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D450" s="2">
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),2.46)</f>
@@ -31221,7 +31252,7 @@
         <v>SULAWESI BARAT</v>
       </c>
       <c r="C451" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D451" s="2">
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),3.72)</f>
@@ -31289,7 +31320,7 @@
         <v>SULAWESI BARAT</v>
       </c>
       <c r="C452" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D452" s="2">
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),2.69)</f>
@@ -31977,9 +32008,8 @@
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"MALUKU")</f>
         <v>MALUKU</v>
       </c>
-      <c r="C462" s="2" t="str">
-        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Ambon")</f>
-        <v>Ambon</v>
+      <c r="C462" s="10" t="s">
+        <v>86</v>
       </c>
       <c r="D462" s="2">
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),12.22)</f>
@@ -32046,9 +32076,8 @@
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"MALUKU")</f>
         <v>MALUKU</v>
       </c>
-      <c r="C463" s="2" t="str">
-        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Tual")</f>
-        <v>Tual</v>
+      <c r="C463" s="10" t="s">
+        <v>91</v>
       </c>
       <c r="D463" s="2">
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),10.91)</f>
@@ -32643,9 +32672,8 @@
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"MALUKU UTARA")</f>
         <v>MALUKU UTARA</v>
       </c>
-      <c r="C472" s="2" t="str">
-        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Ternate")</f>
-        <v>Ternate</v>
+      <c r="C472" s="10" t="s">
+        <v>87</v>
       </c>
       <c r="D472" s="2">
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),5.91)</f>
@@ -32710,7 +32738,7 @@
         <v>MALUKU UTARA</v>
       </c>
       <c r="C473" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D473" s="2">
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),4.97)</f>
@@ -32775,7 +32803,7 @@
         <v>PAPUA BARAT</v>
       </c>
       <c r="C474" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D474" s="2">
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),10.47)</f>
@@ -39305,14 +39333,28 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E27FE57F-1160-4F75-9795-9BADF2FC7FDE}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1:Q5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -39375,7 +39417,7 @@
         <v>9</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="D3" s="7">
         <v>2.72</v>
@@ -39486,7 +39528,7 @@
         <v>9</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="D8" s="7">
         <v>0.75</v>
@@ -39532,7 +39574,7 @@
         <v>20</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D10" s="7">
         <v>9.94</v>

</xml_diff>